<commit_message>
divided values by 12
</commit_message>
<xml_diff>
--- a/regional_simulator/datasheets/big_consumer_consumption_cbr_data.xlsx
+++ b/regional_simulator/datasheets/big_consumer_consumption_cbr_data.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joris\Documents\Fontys\S6\Energy-Grid-Backend\regional_simulator\datasheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D15B567-1CDE-4846-BBE5-D5C84C1C61A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -28,112 +19,110 @@
     <t>yearly_consumption</t>
   </si>
   <si>
-    <t>Sector: Handel</t>
-  </si>
-  <si>
-    <t>Sector: Vervoer en opslag</t>
-  </si>
-  <si>
-    <t>Sector: Horeca</t>
-  </si>
-  <si>
-    <t>Sector: Informatie en communicatie</t>
-  </si>
-  <si>
-    <t>Sector: Financiële dienstverlening</t>
-  </si>
-  <si>
-    <t>Sector: Verhuur en handel van onroerend goed</t>
-  </si>
-  <si>
-    <t>Sector: Specialistische zakelijke diensten</t>
-  </si>
-  <si>
-    <t>Sector: Verhuur en overige zakelijke diensten</t>
-  </si>
-  <si>
-    <t>Sector: Openbaar bestuur en overheidsdiensten</t>
-  </si>
-  <si>
-    <t>Sector: Onderwijs</t>
-  </si>
-  <si>
-    <t>Sector: Gezondheids- en welzijnszorg</t>
-  </si>
-  <si>
-    <t>Sector: Cultuur, sport en recreatie</t>
-  </si>
-  <si>
-    <t>Sector: Overige dienstverlening</t>
-  </si>
-  <si>
-    <t>Sector: Extraterritoriale organisaties</t>
+    <t>Handel</t>
+  </si>
+  <si>
+    <t>Vervoer en opslag</t>
+  </si>
+  <si>
+    <t>Horeca</t>
+  </si>
+  <si>
+    <t>Informatie en communicatie</t>
+  </si>
+  <si>
+    <t>Financiële dienstverlening</t>
+  </si>
+  <si>
+    <t>Verhuur en handel van onroerend goed</t>
+  </si>
+  <si>
+    <t>Specialistische zakelijke diensten</t>
+  </si>
+  <si>
+    <t>Verhuur en overige zakelijke diensten</t>
+  </si>
+  <si>
+    <t>Openbaar bestuur en overheidsdiensten</t>
+  </si>
+  <si>
+    <t>Onderwijs</t>
+  </si>
+  <si>
+    <t>Gezondheids- en welzijnszorg</t>
+  </si>
+  <si>
+    <t>Cultuur, sport en recreatie</t>
+  </si>
+  <si>
+    <t>Overige dienstverlening</t>
+  </si>
+  <si>
+    <t>Extraterritoriale organisaties</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="4">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="4">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -323,29 +312,24 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="31.57"/>
+    <col customWidth="1" min="2" max="2" width="19.29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -353,122 +337,124 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>4597354000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="3">
+        <v>3.831128333333333E8</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
-        <v>4548222000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="3">
+        <v>3.790185E8</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
-        <v>1297757000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="3">
+        <v>1.0814641666666667E8</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
-        <v>2173060000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="3">
+        <v>1.8108833333333334E8</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
-        <v>942452000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="3">
+        <v>7.853766666666667E7</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1">
-        <v>870238000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="3">
+        <v>7.251983333333333E7</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
-        <v>666533000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="3">
+        <v>5.5544416666666664E7</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1">
-        <v>464789000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="3">
+        <v>3.8732416666666664E7</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1">
-        <v>2138478000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" s="3">
+        <v>1.782065E8</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1">
-        <v>1103538000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="3">
+        <v>9.19615E7</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1">
-        <v>2389959000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" s="3">
+        <v>1.9916325E8</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1">
-        <v>909187000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="3">
+        <v>7.576558333333333E7</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1">
-        <v>232490000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" s="3">
+        <v>1.9374166666666668E7</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1">
-        <v>41279000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
+      <c r="B15" s="3">
+        <v>3439916.6666666665</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>